<commit_message>
Analized creating bar plots per age, nationality and sex. (Calculated means and totals per year)
</commit_message>
<xml_diff>
--- a/generated_output/output_condenas_menores.xlsx
+++ b/generated_output/output_condenas_menores.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -417,32 +417,30 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B2" t="n">
+        <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>2911</v>
+        <v>620</v>
       </c>
       <c r="D2" t="n">
-        <v>2824</v>
+        <v>538</v>
       </c>
       <c r="E2" t="n">
-        <v>2582</v>
+        <v>496</v>
       </c>
       <c r="F2" t="n">
-        <v>2840</v>
+        <v>496</v>
       </c>
       <c r="G2" t="n">
-        <v>2901</v>
+        <v>526</v>
       </c>
       <c r="H2" t="n">
-        <v>2756</v>
+        <v>456</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -456,29 +454,29 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>681</v>
+        <v>640</v>
       </c>
       <c r="D3" t="n">
-        <v>607</v>
+        <v>677</v>
       </c>
       <c r="E3" t="n">
-        <v>550</v>
+        <v>583</v>
       </c>
       <c r="F3" t="n">
-        <v>562</v>
+        <v>637</v>
       </c>
       <c r="G3" t="n">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="H3" t="n">
-        <v>550</v>
+        <v>590</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -492,29 +490,29 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>729</v>
+        <v>705</v>
       </c>
       <c r="D4" t="n">
-        <v>760</v>
+        <v>683</v>
       </c>
       <c r="E4" t="n">
-        <v>675</v>
+        <v>617</v>
       </c>
       <c r="F4" t="n">
-        <v>712</v>
+        <v>683</v>
       </c>
       <c r="G4" t="n">
-        <v>710</v>
+        <v>672</v>
       </c>
       <c r="H4" t="n">
-        <v>696</v>
+        <v>642</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -528,29 +526,29 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>794</v>
+        <v>630</v>
       </c>
       <c r="D5" t="n">
-        <v>786</v>
+        <v>587</v>
       </c>
       <c r="E5" t="n">
-        <v>705</v>
+        <v>544</v>
       </c>
       <c r="F5" t="n">
-        <v>786</v>
+        <v>654</v>
       </c>
       <c r="G5" t="n">
-        <v>800</v>
+        <v>640</v>
       </c>
       <c r="H5" t="n">
-        <v>757</v>
+        <v>622</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -564,29 +562,29 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>707</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
-        <v>671</v>
+        <v>26</v>
       </c>
       <c r="E6" t="n">
-        <v>652</v>
+        <v>19</v>
       </c>
       <c r="F6" t="n">
-        <v>780</v>
+        <v>34</v>
       </c>
       <c r="G6" t="n">
-        <v>777</v>
+        <v>34</v>
       </c>
       <c r="H6" t="n">
-        <v>753</v>
+        <v>37</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -599,32 +597,30 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B7" t="n">
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>2595</v>
+        <v>37</v>
       </c>
       <c r="D7" t="n">
-        <v>2485</v>
+        <v>33</v>
       </c>
       <c r="E7" t="n">
-        <v>2240</v>
+        <v>41</v>
       </c>
       <c r="F7" t="n">
-        <v>2470</v>
+        <v>29</v>
       </c>
       <c r="G7" t="n">
-        <v>2449</v>
+        <v>39</v>
       </c>
       <c r="H7" t="n">
-        <v>2310</v>
+        <v>31</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -638,29 +634,29 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>620</v>
+        <v>34</v>
       </c>
       <c r="D8" t="n">
-        <v>538</v>
+        <v>32</v>
       </c>
       <c r="E8" t="n">
-        <v>496</v>
+        <v>39</v>
       </c>
       <c r="F8" t="n">
-        <v>496</v>
+        <v>33</v>
       </c>
       <c r="G8" t="n">
-        <v>526</v>
+        <v>40</v>
       </c>
       <c r="H8" t="n">
-        <v>456</v>
+        <v>32</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -674,29 +670,29 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>640</v>
+        <v>21</v>
       </c>
       <c r="D9" t="n">
-        <v>677</v>
+        <v>35</v>
       </c>
       <c r="E9" t="n">
-        <v>583</v>
+        <v>31</v>
       </c>
       <c r="F9" t="n">
-        <v>637</v>
+        <v>43</v>
       </c>
       <c r="G9" t="n">
-        <v>611</v>
+        <v>47</v>
       </c>
       <c r="H9" t="n">
-        <v>590</v>
+        <v>46</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -710,29 +706,29 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>705</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>683</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>617</v>
+        <v>4</v>
       </c>
       <c r="F10" t="n">
-        <v>683</v>
+        <v>1</v>
       </c>
       <c r="G10" t="n">
-        <v>672</v>
+        <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>642</v>
+        <v>4</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -746,29 +742,29 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>630</v>
+        <v>1</v>
       </c>
       <c r="D11" t="n">
-        <v>587</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>544</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>654</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>640</v>
+        <v>5</v>
       </c>
       <c r="H11" t="n">
-        <v>622</v>
+        <v>7</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -781,32 +777,30 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B12" t="n">
+        <v>16</v>
       </c>
       <c r="C12" t="n">
-        <v>116</v>
+        <v>5</v>
       </c>
       <c r="D12" t="n">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="F12" t="n">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="G12" t="n">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="H12" t="n">
-        <v>146</v>
+        <v>7</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -820,29 +814,29 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D13" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E13" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="G13" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="H13" t="n">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -856,29 +850,29 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D14" t="n">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="E14" t="n">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="F14" t="n">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="G14" t="n">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H14" t="n">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -892,29 +886,29 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E15" t="n">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F15" t="n">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="G15" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="H15" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -928,29 +922,29 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E16" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="F16" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G16" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="H16" t="n">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -963,32 +957,30 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B17" t="n">
+        <v>17</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D17" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E17" t="n">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F17" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G17" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H17" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1005,26 +997,26 @@
         <v>14</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G18" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="H18" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1041,26 +1033,26 @@
         <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F19" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G19" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="H19" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1077,26 +1069,26 @@
         <v>16</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="E20" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F20" t="n">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="G20" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="H20" t="n">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1113,26 +1105,26 @@
         <v>17</v>
       </c>
       <c r="C21" t="n">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D21" t="n">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F21" t="n">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="G21" t="n">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="H21" t="n">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1145,32 +1137,30 @@
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B22" t="n">
+        <v>14</v>
       </c>
       <c r="C22" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="D22" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="F22" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="H22" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de Africa</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1184,29 +1174,29 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E23" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="H23" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de Africa</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1220,29 +1210,29 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C24" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de Africa</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -1256,29 +1246,29 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G25" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="H25" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de Africa</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -1292,29 +1282,29 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C26" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de Africa</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -1327,32 +1317,30 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B27" t="n">
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>118</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="H27" t="n">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De América</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -1366,29 +1354,29 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C28" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De América</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -1402,29 +1390,29 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C29" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De América</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -1438,34 +1426,34 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C30" t="n">
-        <v>28</v>
+        <v>1612</v>
       </c>
       <c r="D30" t="n">
-        <v>29</v>
+        <v>1494</v>
       </c>
       <c r="E30" t="n">
-        <v>30</v>
+        <v>1398</v>
       </c>
       <c r="F30" t="n">
-        <v>48</v>
+        <v>1560</v>
       </c>
       <c r="G30" t="n">
-        <v>60</v>
+        <v>1566</v>
       </c>
       <c r="H30" t="n">
-        <v>55</v>
+        <v>1430</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De América</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1474,34 +1462,34 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C31" t="n">
-        <v>26</v>
+        <v>1898</v>
       </c>
       <c r="D31" t="n">
-        <v>29</v>
+        <v>2000</v>
       </c>
       <c r="E31" t="n">
-        <v>33</v>
+        <v>1950</v>
       </c>
       <c r="F31" t="n">
-        <v>54</v>
+        <v>1978</v>
       </c>
       <c r="G31" t="n">
-        <v>61</v>
+        <v>2089</v>
       </c>
       <c r="H31" t="n">
-        <v>46</v>
+        <v>1974</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De América</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1509,37 +1497,35 @@
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B32" t="n">
+        <v>16</v>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>2456</v>
       </c>
       <c r="D32" t="n">
-        <v>6</v>
+        <v>2400</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2296</v>
       </c>
       <c r="F32" t="n">
-        <v>2</v>
+        <v>2352</v>
       </c>
       <c r="G32" t="n">
-        <v>3</v>
+        <v>2575</v>
       </c>
       <c r="H32" t="n">
-        <v>5</v>
+        <v>2537</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Asia</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1548,34 +1534,34 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>2601</v>
       </c>
       <c r="D33" t="n">
-        <v>1</v>
+        <v>2614</v>
       </c>
       <c r="E33" t="n">
-        <v>1</v>
+        <v>2456</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>2768</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>3085</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>2961</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Asia</t>
+          <t xml:space="preserve">    Española</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1584,34 +1570,34 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="D34" t="n">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>105</v>
       </c>
       <c r="F34" t="n">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="H34" t="n">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Asia</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1620,34 +1606,34 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="D35" t="n">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>164</v>
       </c>
       <c r="H35" t="n">
-        <v>1</v>
+        <v>135</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Asia</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1656,34 +1642,34 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>168</v>
       </c>
       <c r="E36" t="n">
-        <v>1</v>
+        <v>126</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>164</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>159</v>
       </c>
       <c r="H36" t="n">
-        <v>2</v>
+        <v>171</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Asia</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1691,37 +1677,35 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B37" t="n">
+        <v>17</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>148</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>172</v>
       </c>
       <c r="F37" t="n">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="G37" t="n">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>184</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Oceanía</t>
+          <t xml:space="preserve">    País de la Unión Europea sin España</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1733,31 +1717,31 @@
         <v>14</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Oceanía</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1769,31 +1753,31 @@
         <v>15</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Oceanía</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1805,31 +1789,31 @@
         <v>16</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Oceanía</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1841,31 +1825,31 @@
         <v>17</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t xml:space="preserve">    De Oceanía</t>
+          <t xml:space="preserve">    País del resto de Europa</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>mujer</t>
+          <t>hombre</t>
         </is>
       </c>
     </row>
@@ -1873,32 +1857,30 @@
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B42" t="n">
+        <v>14</v>
       </c>
       <c r="C42" t="n">
-        <v>10753</v>
+        <v>137</v>
       </c>
       <c r="D42" t="n">
-        <v>10819</v>
+        <v>170</v>
       </c>
       <c r="E42" t="n">
-        <v>10346</v>
+        <v>134</v>
       </c>
       <c r="F42" t="n">
-        <v>11141</v>
+        <v>117</v>
       </c>
       <c r="G42" t="n">
-        <v>12147</v>
+        <v>157</v>
       </c>
       <c r="H42" t="n">
-        <v>11988</v>
+        <v>154</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -1912,29 +1894,29 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="n">
-        <v>1899</v>
+        <v>256</v>
       </c>
       <c r="D43" t="n">
-        <v>1816</v>
+        <v>235</v>
       </c>
       <c r="E43" t="n">
-        <v>1712</v>
+        <v>229</v>
       </c>
       <c r="F43" t="n">
-        <v>1878</v>
+        <v>222</v>
       </c>
       <c r="G43" t="n">
-        <v>1944</v>
+        <v>237</v>
       </c>
       <c r="H43" t="n">
-        <v>1853</v>
+        <v>263</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -1948,29 +1930,29 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C44" t="n">
-        <v>2351</v>
+        <v>355</v>
       </c>
       <c r="D44" t="n">
-        <v>2457</v>
+        <v>375</v>
       </c>
       <c r="E44" t="n">
-        <v>2444</v>
+        <v>342</v>
       </c>
       <c r="F44" t="n">
-        <v>2494</v>
+        <v>376</v>
       </c>
       <c r="G44" t="n">
-        <v>2706</v>
+        <v>379</v>
       </c>
       <c r="H44" t="n">
-        <v>2627</v>
+        <v>387</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -1984,29 +1966,29 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C45" t="n">
-        <v>3119</v>
+        <v>475</v>
       </c>
       <c r="D45" t="n">
-        <v>3125</v>
+        <v>409</v>
       </c>
       <c r="E45" t="n">
-        <v>2935</v>
+        <v>386</v>
       </c>
       <c r="F45" t="n">
-        <v>3143</v>
+        <v>380</v>
       </c>
       <c r="G45" t="n">
-        <v>3423</v>
+        <v>448</v>
       </c>
       <c r="H45" t="n">
-        <v>3462</v>
+        <v>473</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    País de Africa</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -2020,29 +2002,29 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C46" t="n">
-        <v>3384</v>
+        <v>46</v>
       </c>
       <c r="D46" t="n">
-        <v>3421</v>
+        <v>54</v>
       </c>
       <c r="E46" t="n">
-        <v>3255</v>
+        <v>62</v>
       </c>
       <c r="F46" t="n">
-        <v>3626</v>
+        <v>81</v>
       </c>
       <c r="G46" t="n">
-        <v>4074</v>
+        <v>102</v>
       </c>
       <c r="H46" t="n">
-        <v>4046</v>
+        <v>146</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Total</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -2055,32 +2037,30 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B47" t="n">
+        <v>15</v>
       </c>
       <c r="C47" t="n">
-        <v>8567</v>
+        <v>75</v>
       </c>
       <c r="D47" t="n">
-        <v>8508</v>
+        <v>104</v>
       </c>
       <c r="E47" t="n">
-        <v>8100</v>
+        <v>122</v>
       </c>
       <c r="F47" t="n">
-        <v>8658</v>
+        <v>136</v>
       </c>
       <c r="G47" t="n">
-        <v>9315</v>
+        <v>189</v>
       </c>
       <c r="H47" t="n">
-        <v>8902</v>
+        <v>230</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -2094,29 +2074,29 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C48" t="n">
-        <v>1612</v>
+        <v>146</v>
       </c>
       <c r="D48" t="n">
-        <v>1494</v>
+        <v>148</v>
       </c>
       <c r="E48" t="n">
-        <v>1398</v>
+        <v>152</v>
       </c>
       <c r="F48" t="n">
-        <v>1560</v>
+        <v>224</v>
       </c>
       <c r="G48" t="n">
-        <v>1566</v>
+        <v>279</v>
       </c>
       <c r="H48" t="n">
-        <v>1430</v>
+        <v>338</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
@@ -2130,29 +2110,29 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C49" t="n">
-        <v>1898</v>
+        <v>169</v>
       </c>
       <c r="D49" t="n">
-        <v>2000</v>
+        <v>212</v>
       </c>
       <c r="E49" t="n">
-        <v>1950</v>
+        <v>208</v>
       </c>
       <c r="F49" t="n">
-        <v>1978</v>
+        <v>271</v>
       </c>
       <c r="G49" t="n">
-        <v>2089</v>
+        <v>342</v>
       </c>
       <c r="H49" t="n">
-        <v>1974</v>
+        <v>401</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    De América</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2166,29 +2146,29 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C50" t="n">
-        <v>2456</v>
+        <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>2400</v>
+        <v>10</v>
       </c>
       <c r="E50" t="n">
-        <v>2296</v>
+        <v>4</v>
       </c>
       <c r="F50" t="n">
-        <v>2352</v>
+        <v>2</v>
       </c>
       <c r="G50" t="n">
-        <v>2575</v>
+        <v>5</v>
       </c>
       <c r="H50" t="n">
-        <v>2537</v>
+        <v>7</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -2202,29 +2182,29 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C51" t="n">
-        <v>2601</v>
+        <v>4</v>
       </c>
       <c r="D51" t="n">
-        <v>2614</v>
+        <v>7</v>
       </c>
       <c r="E51" t="n">
-        <v>2456</v>
+        <v>7</v>
       </c>
       <c r="F51" t="n">
-        <v>2768</v>
+        <v>6</v>
       </c>
       <c r="G51" t="n">
-        <v>3085</v>
+        <v>9</v>
       </c>
       <c r="H51" t="n">
-        <v>2961</v>
+        <v>6</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t xml:space="preserve">    Española</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J51" t="inlineStr">
@@ -2237,32 +2217,30 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B52" t="n">
+        <v>16</v>
       </c>
       <c r="C52" t="n">
-        <v>452</v>
+        <v>8</v>
       </c>
       <c r="D52" t="n">
-        <v>500</v>
+        <v>17</v>
       </c>
       <c r="E52" t="n">
-        <v>529</v>
+        <v>10</v>
       </c>
       <c r="F52" t="n">
-        <v>604</v>
+        <v>9</v>
       </c>
       <c r="G52" t="n">
-        <v>580</v>
+        <v>8</v>
       </c>
       <c r="H52" t="n">
-        <v>599</v>
+        <v>12</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
@@ -2276,29 +2254,29 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C53" t="n">
-        <v>90</v>
+        <v>9</v>
       </c>
       <c r="D53" t="n">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="E53" t="n">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="F53" t="n">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="G53" t="n">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="H53" t="n">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    De Asia</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
@@ -2312,29 +2290,29 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C54" t="n">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="F54" t="n">
-        <v>143</v>
+        <v>1</v>
       </c>
       <c r="G54" t="n">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
@@ -2348,29 +2326,29 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C55" t="n">
-        <v>143</v>
+        <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>168</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="F55" t="n">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>159</v>
+        <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>171</v>
+        <v>1</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -2384,29 +2362,29 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C56" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>148</v>
+        <v>1</v>
       </c>
       <c r="E56" t="n">
-        <v>172</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>184</v>
+        <v>0</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País de la Unión Europea sin España</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -2419,907 +2397,33 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
+      <c r="B57" t="n">
+        <v>17</v>
       </c>
       <c r="C57" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
+          <t xml:space="preserve">    De Oceanía</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="n">
-        <v>14</v>
-      </c>
-      <c r="C58" t="n">
-        <v>13</v>
-      </c>
-      <c r="D58" t="n">
-        <v>6</v>
-      </c>
-      <c r="E58" t="n">
-        <v>9</v>
-      </c>
-      <c r="F58" t="n">
-        <v>4</v>
-      </c>
-      <c r="G58" t="n">
-        <v>13</v>
-      </c>
-      <c r="H58" t="n">
-        <v>6</v>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="n">
-        <v>15</v>
-      </c>
-      <c r="C59" t="n">
-        <v>9</v>
-      </c>
-      <c r="D59" t="n">
-        <v>8</v>
-      </c>
-      <c r="E59" t="n">
-        <v>10</v>
-      </c>
-      <c r="F59" t="n">
-        <v>9</v>
-      </c>
-      <c r="G59" t="n">
-        <v>18</v>
-      </c>
-      <c r="H59" t="n">
-        <v>18</v>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="n">
-        <v>16</v>
-      </c>
-      <c r="C60" t="n">
-        <v>11</v>
-      </c>
-      <c r="D60" t="n">
-        <v>16</v>
-      </c>
-      <c r="E60" t="n">
-        <v>9</v>
-      </c>
-      <c r="F60" t="n">
-        <v>18</v>
-      </c>
-      <c r="G60" t="n">
-        <v>23</v>
-      </c>
-      <c r="H60" t="n">
-        <v>17</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="n">
-        <v>17</v>
-      </c>
-      <c r="C61" t="n">
-        <v>19</v>
-      </c>
-      <c r="D61" t="n">
-        <v>26</v>
-      </c>
-      <c r="E61" t="n">
-        <v>28</v>
-      </c>
-      <c r="F61" t="n">
-        <v>17</v>
-      </c>
-      <c r="G61" t="n">
-        <v>32</v>
-      </c>
-      <c r="H61" t="n">
-        <v>19</v>
-      </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País del resto de Europa</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
-      </c>
-      <c r="C62" t="n">
-        <v>1223</v>
-      </c>
-      <c r="D62" t="n">
-        <v>1189</v>
-      </c>
-      <c r="E62" t="n">
-        <v>1091</v>
-      </c>
-      <c r="F62" t="n">
-        <v>1095</v>
-      </c>
-      <c r="G62" t="n">
-        <v>1221</v>
-      </c>
-      <c r="H62" t="n">
-        <v>1277</v>
-      </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País de Africa</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="B63" t="n">
-        <v>14</v>
-      </c>
-      <c r="C63" t="n">
-        <v>137</v>
-      </c>
-      <c r="D63" t="n">
-        <v>170</v>
-      </c>
-      <c r="E63" t="n">
-        <v>134</v>
-      </c>
-      <c r="F63" t="n">
-        <v>117</v>
-      </c>
-      <c r="G63" t="n">
-        <v>157</v>
-      </c>
-      <c r="H63" t="n">
-        <v>154</v>
-      </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País de Africa</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="B64" t="n">
-        <v>15</v>
-      </c>
-      <c r="C64" t="n">
-        <v>256</v>
-      </c>
-      <c r="D64" t="n">
-        <v>235</v>
-      </c>
-      <c r="E64" t="n">
-        <v>229</v>
-      </c>
-      <c r="F64" t="n">
-        <v>222</v>
-      </c>
-      <c r="G64" t="n">
-        <v>237</v>
-      </c>
-      <c r="H64" t="n">
-        <v>263</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País de Africa</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="B65" t="n">
-        <v>16</v>
-      </c>
-      <c r="C65" t="n">
-        <v>355</v>
-      </c>
-      <c r="D65" t="n">
-        <v>375</v>
-      </c>
-      <c r="E65" t="n">
-        <v>342</v>
-      </c>
-      <c r="F65" t="n">
-        <v>376</v>
-      </c>
-      <c r="G65" t="n">
-        <v>379</v>
-      </c>
-      <c r="H65" t="n">
-        <v>387</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País de Africa</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="B66" t="n">
-        <v>17</v>
-      </c>
-      <c r="C66" t="n">
-        <v>475</v>
-      </c>
-      <c r="D66" t="n">
-        <v>409</v>
-      </c>
-      <c r="E66" t="n">
-        <v>386</v>
-      </c>
-      <c r="F66" t="n">
-        <v>380</v>
-      </c>
-      <c r="G66" t="n">
-        <v>448</v>
-      </c>
-      <c r="H66" t="n">
-        <v>473</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    País de Africa</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>436</v>
-      </c>
-      <c r="D67" t="n">
-        <v>518</v>
-      </c>
-      <c r="E67" t="n">
-        <v>544</v>
-      </c>
-      <c r="F67" t="n">
-        <v>712</v>
-      </c>
-      <c r="G67" t="n">
-        <v>912</v>
-      </c>
-      <c r="H67" t="n">
-        <v>1115</v>
-      </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De América</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="n">
-        <v>14</v>
-      </c>
-      <c r="C68" t="n">
-        <v>46</v>
-      </c>
-      <c r="D68" t="n">
-        <v>54</v>
-      </c>
-      <c r="E68" t="n">
-        <v>62</v>
-      </c>
-      <c r="F68" t="n">
-        <v>81</v>
-      </c>
-      <c r="G68" t="n">
-        <v>102</v>
-      </c>
-      <c r="H68" t="n">
-        <v>146</v>
-      </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De América</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="n">
-        <v>15</v>
-      </c>
-      <c r="C69" t="n">
-        <v>75</v>
-      </c>
-      <c r="D69" t="n">
-        <v>104</v>
-      </c>
-      <c r="E69" t="n">
-        <v>122</v>
-      </c>
-      <c r="F69" t="n">
-        <v>136</v>
-      </c>
-      <c r="G69" t="n">
-        <v>189</v>
-      </c>
-      <c r="H69" t="n">
-        <v>230</v>
-      </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De América</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="n">
-        <v>16</v>
-      </c>
-      <c r="C70" t="n">
-        <v>146</v>
-      </c>
-      <c r="D70" t="n">
-        <v>148</v>
-      </c>
-      <c r="E70" t="n">
-        <v>152</v>
-      </c>
-      <c r="F70" t="n">
-        <v>224</v>
-      </c>
-      <c r="G70" t="n">
-        <v>279</v>
-      </c>
-      <c r="H70" t="n">
-        <v>338</v>
-      </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De América</t>
-        </is>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="n">
-        <v>17</v>
-      </c>
-      <c r="C71" t="n">
-        <v>169</v>
-      </c>
-      <c r="D71" t="n">
-        <v>212</v>
-      </c>
-      <c r="E71" t="n">
-        <v>208</v>
-      </c>
-      <c r="F71" t="n">
-        <v>271</v>
-      </c>
-      <c r="G71" t="n">
-        <v>342</v>
-      </c>
-      <c r="H71" t="n">
-        <v>401</v>
-      </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De América</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
-      </c>
-      <c r="C72" t="n">
-        <v>22</v>
-      </c>
-      <c r="D72" t="n">
-        <v>46</v>
-      </c>
-      <c r="E72" t="n">
-        <v>26</v>
-      </c>
-      <c r="F72" t="n">
-        <v>23</v>
-      </c>
-      <c r="G72" t="n">
-        <v>33</v>
-      </c>
-      <c r="H72" t="n">
-        <v>33</v>
-      </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Asia</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="n">
-        <v>14</v>
-      </c>
-      <c r="C73" t="n">
-        <v>1</v>
-      </c>
-      <c r="D73" t="n">
-        <v>10</v>
-      </c>
-      <c r="E73" t="n">
-        <v>4</v>
-      </c>
-      <c r="F73" t="n">
-        <v>2</v>
-      </c>
-      <c r="G73" t="n">
-        <v>5</v>
-      </c>
-      <c r="H73" t="n">
-        <v>7</v>
-      </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Asia</t>
-        </is>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="n">
-        <v>15</v>
-      </c>
-      <c r="C74" t="n">
-        <v>4</v>
-      </c>
-      <c r="D74" t="n">
-        <v>7</v>
-      </c>
-      <c r="E74" t="n">
-        <v>7</v>
-      </c>
-      <c r="F74" t="n">
-        <v>6</v>
-      </c>
-      <c r="G74" t="n">
-        <v>9</v>
-      </c>
-      <c r="H74" t="n">
-        <v>6</v>
-      </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Asia</t>
-        </is>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="n">
-        <v>16</v>
-      </c>
-      <c r="C75" t="n">
-        <v>8</v>
-      </c>
-      <c r="D75" t="n">
-        <v>17</v>
-      </c>
-      <c r="E75" t="n">
-        <v>10</v>
-      </c>
-      <c r="F75" t="n">
-        <v>9</v>
-      </c>
-      <c r="G75" t="n">
-        <v>8</v>
-      </c>
-      <c r="H75" t="n">
-        <v>12</v>
-      </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Asia</t>
-        </is>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="n">
-        <v>17</v>
-      </c>
-      <c r="C76" t="n">
-        <v>9</v>
-      </c>
-      <c r="D76" t="n">
-        <v>12</v>
-      </c>
-      <c r="E76" t="n">
-        <v>5</v>
-      </c>
-      <c r="F76" t="n">
-        <v>6</v>
-      </c>
-      <c r="G76" t="n">
-        <v>11</v>
-      </c>
-      <c r="H76" t="n">
-        <v>8</v>
-      </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Asia</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                Total</t>
-        </is>
-      </c>
-      <c r="C77" t="n">
-        <v>1</v>
-      </c>
-      <c r="D77" t="n">
-        <v>2</v>
-      </c>
-      <c r="E77" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G77" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" t="n">
-        <v>2</v>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Oceanía</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" s="1" t="n">
-        <v>76</v>
-      </c>
-      <c r="B78" t="n">
-        <v>14</v>
-      </c>
-      <c r="C78" t="n">
-        <v>0</v>
-      </c>
-      <c r="D78" t="n">
-        <v>1</v>
-      </c>
-      <c r="E78" t="n">
-        <v>0</v>
-      </c>
-      <c r="F78" t="n">
-        <v>1</v>
-      </c>
-      <c r="G78" t="n">
-        <v>0</v>
-      </c>
-      <c r="H78" t="n">
-        <v>1</v>
-      </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Oceanía</t>
-        </is>
-      </c>
-      <c r="J78" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" s="1" t="n">
-        <v>77</v>
-      </c>
-      <c r="B79" t="n">
-        <v>15</v>
-      </c>
-      <c r="C79" t="n">
-        <v>0</v>
-      </c>
-      <c r="D79" t="n">
-        <v>0</v>
-      </c>
-      <c r="E79" t="n">
-        <v>0</v>
-      </c>
-      <c r="F79" t="n">
-        <v>0</v>
-      </c>
-      <c r="G79" t="n">
-        <v>0</v>
-      </c>
-      <c r="H79" t="n">
-        <v>1</v>
-      </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Oceanía</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="B80" t="n">
-        <v>16</v>
-      </c>
-      <c r="C80" t="n">
-        <v>0</v>
-      </c>
-      <c r="D80" t="n">
-        <v>1</v>
-      </c>
-      <c r="E80" t="n">
-        <v>0</v>
-      </c>
-      <c r="F80" t="n">
-        <v>0</v>
-      </c>
-      <c r="G80" t="n">
-        <v>0</v>
-      </c>
-      <c r="H80" t="n">
-        <v>0</v>
-      </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Oceanía</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>hombre</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="B81" t="n">
-        <v>17</v>
-      </c>
-      <c r="C81" t="n">
-        <v>1</v>
-      </c>
-      <c r="D81" t="n">
-        <v>0</v>
-      </c>
-      <c r="E81" t="n">
-        <v>0</v>
-      </c>
-      <c r="F81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G81" t="n">
-        <v>0</v>
-      </c>
-      <c r="H81" t="n">
-        <v>0</v>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t xml:space="preserve">    De Oceanía</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
         <is>
           <t>hombre</t>
         </is>

</xml_diff>

<commit_message>
Finished preparing and analyzing data2
</commit_message>
<xml_diff>
--- a/generated_output/output_condenas_menores.xlsx
+++ b/generated_output/output_condenas_menores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -9130,6 +9130,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>